<commit_message>
Atualização do arquivo de planilhas
</commit_message>
<xml_diff>
--- a/05_contPlanilhas.xlsx
+++ b/05_contPlanilhas.xlsx
@@ -1310,13 +1310,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D101BFC-D9D9-48F5-BFF6-C1B2AE60AEE0}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{468E01C8-DF0E-4120-8BD2-C2C47612EC6A}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C1C33EF-4614-467D-B19E-D4D15600261D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1EEA9AEA-C297-44CB-B11E-F4AA05AC2FB3}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{822ABAED-23F3-49CD-89B6-3AFB1B546F29}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2618323-4B1E-4FC1-B74C-F8871E8433AF}"/>
 </file>
</xml_diff>